<commit_message>
Fixes Wait Time validation for min/max/period inputs
display.php and displayInterface.php have been updated to insert an invisible submit button into the form.

updateDisplay() now correctly performs form validation on any inputs that have constraints.

Pattern attribute was added to ticket creation's nickname input field to only accept numbers and letters. This eliminates SQL injection for this input when the document is not edited through debug.
</commit_message>
<xml_diff>
--- a/Sprint2Demo/Sprint2DemoScript.xlsx
+++ b/Sprint2Demo/Sprint2DemoScript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Sprint2Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23018D0E-A3D0-4B92-A6D7-30BD8EE9F9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2814D00-6B99-4F1C-A1A2-049CA0BB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{076E1F84-F2C5-44D5-AA4F-87672F907B8E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{076E1F84-F2C5-44D5-AA4F-87672F907B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>Feature Demonstrated</t>
   </si>
@@ -377,12 +377,18 @@
   <si>
     <t>Explain that parties pay at front, and currently that process will remove the ticket form the table automatically, and not kick the ticket back to the Wait List. Will change on future sprint/ Phase 2</t>
   </si>
+  <si>
+    <t>CentRes Point of sale Solution    SPRINT 2 DEMO : HOST VIEW / MANAGER VIEW &amp; FUNCTIONS</t>
+  </si>
+  <si>
+    <t>CentRes Point of sale Solution : SPRINT 2 DEMO : HostView/ManagerView/Manager Functions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +428,14 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1047,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1230,6 +1244,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1287,55 +1352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1652,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D7DE53-073D-4EF7-966D-7E5F76C87298}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1670,583 +1687,593 @@
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="76" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="75" t="s">
+      <c r="F2" s="94"/>
+      <c r="G2" s="92" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="70"/>
-      <c r="B2" s="10" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="87"/>
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="75"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="81"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="G3" s="92"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="62"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="7" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="82" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B5" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="83"/>
-      <c r="B5" s="41" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="64"/>
+      <c r="B6" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D6" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="84"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="60" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="65"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="22" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="82"/>
-      <c r="B7" s="38" t="s">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="63"/>
+      <c r="B8" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="65" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="82"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="66"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="82"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="38"/>
       <c r="C9" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D9" s="40"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="66"/>
+      <c r="F9" s="83"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="82"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="38"/>
       <c r="C10" s="39" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="66"/>
+      <c r="F10" s="83"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="82"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="38"/>
       <c r="C11" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="40"/>
+        <v>83</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="66"/>
+      <c r="F11" s="83"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="82"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="38"/>
       <c r="C12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="63"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D13" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="83"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="64"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="85"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48" t="s">
+      <c r="F14" s="84"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="66"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D15" s="49" t="s">
         <v>23</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="82"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="82"/>
-      <c r="B16" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="A16" s="63"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="39" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="63"/>
+      <c r="B17" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="82"/>
-      <c r="B17" s="78" t="s">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="63"/>
+      <c r="B18" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C18" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="82"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>24</v>
-      </c>
+      <c r="D18" s="40"/>
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="82"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="39" t="s">
+        <v>16</v>
+      </c>
       <c r="D19" s="40" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="18"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="86" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="63"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B21" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C21" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D21" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="87"/>
-      <c r="B21" s="79" t="s">
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="68"/>
+      <c r="B22" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C22" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D22" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="71" t="s">
+      <c r="E22" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="63"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="88"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="39" t="s">
+      <c r="F22" s="80"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="69"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="86"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="50" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="67"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="89"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45" t="s">
+      <c r="D24" s="43"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="70"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="72" t="s">
+      <c r="D25" s="46"/>
+      <c r="E25" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="73"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="86"/>
-      <c r="B25" s="51" t="s">
+      <c r="F25" s="90"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="67"/>
+      <c r="B26" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C26" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D26" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="87"/>
-      <c r="B26" s="47" t="s">
+      <c r="E26" s="91"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="68"/>
+      <c r="B27" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C27" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D27" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="88"/>
-      <c r="B27" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="40"/>
       <c r="E27" s="5"/>
       <c r="F27" s="4"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="88"/>
-      <c r="B28" s="38"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="69"/>
+      <c r="B28" s="38" t="s">
+        <v>76</v>
+      </c>
       <c r="C28" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>74</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="4"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="86"/>
-      <c r="B29" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="20"/>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="69"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>74</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="89"/>
-      <c r="B30" s="44" t="s">
+    <row r="30" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="67"/>
+      <c r="B30" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="70"/>
+      <c r="B31" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C31" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D31" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="21" t="s">
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="86"/>
-      <c r="B31" s="41" t="s">
+    <row r="32" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="67"/>
+      <c r="B32" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C32" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D32" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="68" t="s">
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="85" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="90" t="s">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B33" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="56" t="s">
+      <c r="C33" s="48"/>
+      <c r="D33" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E33" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="68"/>
-    </row>
-    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="91"/>
-      <c r="B33" s="38" t="s">
+      <c r="F33" s="18"/>
+      <c r="G33" s="85"/>
+    </row>
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="72"/>
+      <c r="B34" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C34" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="D34" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="68"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="92"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="43"/>
       <c r="E34" s="16"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="68"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="93" t="s">
+      <c r="G34" s="85"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="73"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="43"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="85"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B36" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C36" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="29" t="s">
+      <c r="D36" s="49"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="94"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="16"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="62" t="s">
-        <v>61</v>
-      </c>
-    </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="94"/>
+      <c r="A37" s="75"/>
       <c r="B37" s="38"/>
       <c r="C37" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="40"/>
+        <v>62</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>63</v>
+      </c>
       <c r="E37" s="16"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="63"/>
+      <c r="G37" s="79" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="94"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="38"/>
       <c r="C38" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>67</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D38" s="40"/>
       <c r="E38" s="16"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="63"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="95"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="59" t="s">
+      <c r="G38" s="80"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="75"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="80"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="76"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D40" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="64"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="97" t="s">
+      <c r="E40" s="25"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="81"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="78" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="61" t="s">
+    <row r="42" spans="1:7" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A43" s="61" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="F7:F13"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="F8:F14"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E22:F24"/>
+    <mergeCell ref="E25:F26"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>